<commit_message>
add regex to find product name amount
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>barkod</t>
   </si>
@@ -41,6 +41,30 @@
   </si>
   <si>
     <t>rakip ortalama satis fiyati</t>
+  </si>
+  <si>
+    <t>CASTROL EDGE 5W/40 1LT TU</t>
+  </si>
+  <si>
+    <t>Castrol</t>
+  </si>
+  <si>
+    <t>MADENİ YAĞLAR</t>
+  </si>
+  <si>
+    <t>ad</t>
+  </si>
+  <si>
+    <t>CASTROL EDGE 5W40 4 LT</t>
+  </si>
+  <si>
+    <t>CASTROL EDGE SUPERCAR TU 10W-60 4LT</t>
+  </si>
+  <si>
+    <t>CASTROL ENGİNE SHAMPOO DİESEL 300 ML</t>
+  </si>
+  <si>
+    <t>Oto Bakım</t>
   </si>
 </sst>
 </file>
@@ -417,7 +441,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -450,6 +474,122 @@
       </c>
       <c r="J1" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>8692768038931</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <v>77</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2">
+        <v>315.006</v>
+      </c>
+      <c r="J2">
+        <v>315.006</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>4008177151385</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3">
+        <v>513.7</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3">
+        <v>973.9403703703703</v>
+      </c>
+      <c r="J3">
+        <v>973.9403703703703</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4008177132476</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4">
+        <v>729.3</v>
+      </c>
+      <c r="G4">
+        <v>21</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4">
+        <v>1018.794</v>
+      </c>
+      <c r="J4">
+        <v>1018.794</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4008177157134</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5">
+        <v>38.5</v>
+      </c>
+      <c r="G5">
+        <v>34</v>
+      </c>
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5">
+        <v>117</v>
+      </c>
+      <c r="J5">
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
try to fix to filter scraped product data
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -499,10 +499,10 @@
         <v>13</v>
       </c>
       <c r="I2">
-        <v>315.006</v>
+        <v>291</v>
       </c>
       <c r="J2">
-        <v>315.006</v>
+        <v>291</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -528,10 +528,10 @@
         <v>13</v>
       </c>
       <c r="I3">
-        <v>973.9403703703703</v>
+        <v>960.8647826086956</v>
       </c>
       <c r="J3">
-        <v>973.9403703703703</v>
+        <v>960.8647826086956</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -557,10 +557,10 @@
         <v>13</v>
       </c>
       <c r="I4">
-        <v>1018.794</v>
+        <v>1022.195</v>
       </c>
       <c r="J4">
-        <v>1018.794</v>
+        <v>1022.195</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>